<commit_message>
commit previous to fedora update
</commit_message>
<xml_diff>
--- a/mdaher.xlsx
+++ b/mdaher.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Octubre" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Noviembre" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Diciembre" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Diciembre_Horas" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Diciembre_Objetivos" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
   <si>
     <t xml:space="preserve">Octubre</t>
   </si>
@@ -150,7 +151,64 @@
     <t xml:space="preserve">Instalar actualizaciones y empezar excel.</t>
   </si>
   <si>
-    <t xml:space="preserve">HOY</t>
+    <t xml:space="preserve">Cuentas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPICYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laurus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosas que se hicieron en diciembre pero se perdió información:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venta IPICYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Github y AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reisntalar OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venta Tonalá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contratar Github y AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinstalar OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diciembre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objetivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdataa.com → AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facturas Daniel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual rdataa.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual rdataa.com/aanalyzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdataa.com/profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdataa.com/profile/licences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdataa.com/profile/support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdataa.com /profile/my_account</t>
   </si>
 </sst>
 </file>
@@ -165,6 +223,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -186,15 +245,17 @@
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,6 +284,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2BD27E"/>
         <bgColor rgb="FF3FBE3F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -267,7 +334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,6 +369,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -685,7 +756,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1012,7 +1083,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1025,15 +1096,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,11 +1202,23 @@
       <c r="B7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="C7" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="4"/>
+      <c r="H7" s="0" t="n">
+        <f aca="false">SUM(C7:G7)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -1143,10 +1228,17 @@
       <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
+      <c r="I8" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -1170,24 +1262,64 @@
       <c r="G9" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="I9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="B10" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>5.5</v>
+      </c>
       <c r="G10" s="4"/>
+      <c r="H10" s="0" t="n">
+        <f aca="false">SUM(A10:G10)</f>
+        <v>19.5</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="G11" s="5"/>
+      <c r="I11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -1210,6 +1342,12 @@
       </c>
       <c r="G12" s="3" t="n">
         <v>23</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,6 +1419,18 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
+      <c r="I18" s="0" t="n">
+        <f aca="false">H7+H10</f>
+        <v>36.5</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">(6000/21)/8</f>
+        <v>35.7142857142857</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <f aca="false">I18*J18</f>
+        <v>1303.57142857143</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
@@ -1306,7 +1456,242 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AF19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="2" style="0" width="2.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="33" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="U2" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W2" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="X2" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="3" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>